<commit_message>
Added db schema and seeding it
</commit_message>
<xml_diff>
--- a/src/data/CoursesPrograms/Financials.xlsx
+++ b/src/data/CoursesPrograms/Financials.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27628"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C86398FC-D059-429F-9269-923FE64F23A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{195953E3-6C7A-4E77-8347-F8289C69A2CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Analiza Finansowa" sheetId="1" r:id="rId1"/>
@@ -858,7 +858,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B74"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
+    <sheetView topLeftCell="A23" workbookViewId="0">
       <selection activeCell="B72" sqref="B72"/>
     </sheetView>
   </sheetViews>
@@ -1096,8 +1096,8 @@
       <c r="A29" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B29" s="8" t="s">
-        <v>41</v>
+      <c r="B29" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -1176,8 +1176,8 @@
       <c r="A39" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B39" s="8" t="s">
-        <v>41</v>
+      <c r="B39" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -1200,8 +1200,8 @@
       <c r="A42" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="B42" s="8" t="s">
-        <v>41</v>
+      <c r="B42" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -1360,8 +1360,8 @@
       <c r="A62" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="B62" s="8" t="s">
-        <v>41</v>
+      <c r="B62" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
@@ -1440,8 +1440,8 @@
       <c r="A72" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="B72" s="8" t="s">
-        <v>41</v>
+      <c r="B72" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
@@ -1470,8 +1470,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>